<commit_message>
fix belt profile name
</commit_message>
<xml_diff>
--- a/byo/bom.xlsx
+++ b/byo/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\_vt\strawlab\projects\flo-hardware\byo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BEC56C-1AE4-4047-BEA4-8F7B8ED5358A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5A56DB-67A3-4CDE-95A3-E8AA80FFD5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2480" yWindow="2440" windowWidth="25600" windowHeight="11270" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="25600" windowHeight="11270" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>belt (tilt)</t>
   </si>
   <si>
-    <t>MXL profile 2mm/tooth 110 teeth 5mm width</t>
-  </si>
-  <si>
     <t>??</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>belt (pan)</t>
   </si>
   <si>
-    <t>MXL profile 2mm/tooth 256 teeth 6.5mm width</t>
-  </si>
-  <si>
     <t>880MXL</t>
   </si>
   <si>
@@ -772,6 +766,12 @@
   </si>
   <si>
     <t>byo/focusing/36jx30k5.18-mount.FCStd</t>
+  </si>
+  <si>
+    <t>GT2 profile 110 teeth 5mm width</t>
+  </si>
+  <si>
+    <t>GT2 profile 256 teeth 6.5mm width</t>
   </si>
 </sst>
 </file>
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25A315E-DF31-4262-87C2-ADD015BB9516}">
   <dimension ref="A9:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1210,7 +1210,7 @@
         <v>32</v>
       </c>
       <c r="L9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
@@ -1666,16 +1666,16 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>92</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
@@ -1689,13 +1689,13 @@
         <v>87</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>88</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
@@ -1706,124 +1706,124 @@
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
       </c>
       <c r="D36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
       </c>
       <c r="D38" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F38" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
         <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E40" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F40" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
         <v>83</v>
       </c>
       <c r="F41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -1831,76 +1831,76 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J42" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
         <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
         <v>31</v>
       </c>
       <c r="D44" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="J44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
       </c>
       <c r="D45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" t="s">
         <v>116</v>
-      </c>
-      <c r="E45" t="s">
-        <v>117</v>
-      </c>
-      <c r="F45" t="s">
-        <v>118</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -1908,19 +1908,19 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
       </c>
       <c r="D46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46" t="s">
         <v>119</v>
-      </c>
-      <c r="E46" t="s">
-        <v>120</v>
-      </c>
-      <c r="F46" t="s">
-        <v>121</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -1928,174 +1928,174 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
         <v>29</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
         <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
         <v>29</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E49" t="s">
         <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G49">
         <v>4</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
         <v>29</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
         <v>26</v>
       </c>
       <c r="F50" t="s">
+        <v>125</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E51" t="s">
         <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E52" t="s">
         <v>26</v>
       </c>
       <c r="F52" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C53" t="s">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E53" t="s">
         <v>26</v>
       </c>
       <c r="F53" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
         <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E54" t="s">
         <v>26</v>
       </c>
       <c r="F54" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G54">
         <v>3</v>
@@ -2103,19 +2103,19 @@
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
         <v>29</v>
       </c>
       <c r="D55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E55" t="s">
         <v>26</v>
       </c>
       <c r="F55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2123,19 +2123,19 @@
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
       </c>
       <c r="D56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E56" t="s">
         <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -2143,134 +2143,134 @@
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K57" t="s">
         <v>61</v>
       </c>
       <c r="L57" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
         <v>39</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K58" t="s">
         <v>61</v>
       </c>
       <c r="L58" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C59" t="s">
         <v>39</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K59" t="s">
         <v>61</v>
       </c>
       <c r="L59" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C60" t="s">
         <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K60" t="s">
         <v>61</v>
       </c>
       <c r="L60" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
       </c>
       <c r="D61" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G61">
         <v>2</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K61" t="s">
         <v>61</v>
       </c>
       <c r="L61" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C62" t="s">
         <v>39</v>
       </c>
       <c r="D62" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E62" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F62" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G62">
         <v>2</v>
@@ -2279,24 +2279,24 @@
         <v>61</v>
       </c>
       <c r="L62" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C63" t="s">
         <v>39</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F63" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G63">
         <v>3</v>
@@ -2305,18 +2305,18 @@
         <v>61</v>
       </c>
       <c r="L63" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C64" t="s">
         <v>39</v>
       </c>
       <c r="D64" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G64">
         <v>2</v>
@@ -2325,24 +2325,24 @@
         <v>61</v>
       </c>
       <c r="L64" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C65" t="s">
         <v>39</v>
       </c>
       <c r="D65" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E65" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G65">
         <v>1</v>
@@ -2351,70 +2351,70 @@
         <v>61</v>
       </c>
       <c r="L65" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C66" t="s">
         <v>39</v>
       </c>
       <c r="D66" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G66">
         <v>2</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K66" t="s">
         <v>61</v>
       </c>
       <c r="L66" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C67" t="s">
         <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G67">
         <v>2</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K67" t="s">
         <v>61</v>
       </c>
       <c r="L67" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C68" t="s">
         <v>39</v>
       </c>
       <c r="D68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E68" t="s">
         <v>79</v>
       </c>
       <c r="F68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -2423,24 +2423,24 @@
         <v>61</v>
       </c>
       <c r="L68" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
         <v>39</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E69" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F69" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -2449,18 +2449,18 @@
         <v>61</v>
       </c>
       <c r="L69" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C70" t="s">
         <v>39</v>
       </c>
       <c r="D70" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -2469,18 +2469,18 @@
         <v>61</v>
       </c>
       <c r="L70" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C71" t="s">
         <v>39</v>
       </c>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -2489,18 +2489,18 @@
         <v>61</v>
       </c>
       <c r="L71" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C72" t="s">
         <v>39</v>
       </c>
       <c r="D72" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -2509,24 +2509,24 @@
         <v>61</v>
       </c>
       <c r="L72" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
       </c>
       <c r="D73" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F73" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G73">
         <v>1</v>
@@ -2535,18 +2535,18 @@
         <v>61</v>
       </c>
       <c r="L73" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
       </c>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G74">
         <v>4</v>
@@ -2555,18 +2555,18 @@
         <v>61</v>
       </c>
       <c r="L74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C75" t="s">
         <v>39</v>
       </c>
       <c r="D75" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G75">
         <v>9</v>
@@ -2575,18 +2575,18 @@
         <v>61</v>
       </c>
       <c r="L75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G76">
         <v>2</v>
@@ -2595,18 +2595,18 @@
         <v>61</v>
       </c>
       <c r="L76" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C77" t="s">
         <v>39</v>
       </c>
       <c r="D77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -2615,18 +2615,18 @@
         <v>61</v>
       </c>
       <c r="L77" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
       </c>
       <c r="D78" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -2635,24 +2635,24 @@
         <v>61</v>
       </c>
       <c r="L78" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
       </c>
       <c r="D79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G79">
         <v>1</v>
@@ -2661,24 +2661,24 @@
         <v>61</v>
       </c>
       <c r="L79" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C80" t="s">
         <v>39</v>
       </c>
       <c r="D80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E80" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F80" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -2687,24 +2687,24 @@
         <v>61</v>
       </c>
       <c r="L80" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C81" t="s">
         <v>39</v>
       </c>
       <c r="D81" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E81" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F81" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G81">
         <v>1</v>
@@ -2713,24 +2713,24 @@
         <v>61</v>
       </c>
       <c r="L81" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C82" t="s">
         <v>39</v>
       </c>
       <c r="D82" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E82" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F82" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -2739,7 +2739,7 @@
         <v>61</v>
       </c>
       <c r="L82" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 3d print parts
</commit_message>
<xml_diff>
--- a/byo/bom.xlsx
+++ b/byo/bom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\_vt\strawlab\projects\flo-hardware\byo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thanglam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5A56DB-67A3-4CDE-95A3-E8AA80FFD5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556CA13B-31DA-4516-9419-6A951D3ADE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="25600" windowHeight="11270" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="328">
   <si>
     <t>no</t>
   </si>
@@ -279,9 +279,6 @@
     <t>XT30U</t>
   </si>
   <si>
-    <t>tracking/moving-mirror</t>
-  </si>
-  <si>
     <t>smart stepper</t>
   </si>
   <si>
@@ -324,18 +321,9 @@
     <t>bottom mirror frame</t>
   </si>
   <si>
-    <t>1-st surface mirror, 108*140mm, 3mm thickness</t>
-  </si>
-  <si>
     <t>hot mirror</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>mirror that only reflects IR</t>
-  </si>
-  <si>
     <t>hot mirror frame</t>
   </si>
   <si>
@@ -772,6 +760,264 @@
   </si>
   <si>
     <t>GT2 profile 256 teeth 6.5mm width</t>
+  </si>
+  <si>
+    <t>C mount to Fmount adapter</t>
+  </si>
+  <si>
+    <t>byo/pantilt</t>
+  </si>
+  <si>
+    <t>Pan motor pulley</t>
+  </si>
+  <si>
+    <t>Pan motor plate</t>
+  </si>
+  <si>
+    <t>Pan motor stopper</t>
+  </si>
+  <si>
+    <t>Pan rotor</t>
+  </si>
+  <si>
+    <t>Pan base</t>
+  </si>
+  <si>
+    <t>Pan bearing stopper bottom</t>
+  </si>
+  <si>
+    <t>Pan bearing stopper top</t>
+  </si>
+  <si>
+    <t>Tilt base</t>
+  </si>
+  <si>
+    <t>Tilt motor base</t>
+  </si>
+  <si>
+    <t>Tilt motor pulley</t>
+  </si>
+  <si>
+    <t>Tilt motor spacer</t>
+  </si>
+  <si>
+    <t>Tilt bearing stopper</t>
+  </si>
+  <si>
+    <t>Pantilt head cover</t>
+  </si>
+  <si>
+    <t>Pan tensioner knot</t>
+  </si>
+  <si>
+    <t>Tilt bearing</t>
+  </si>
+  <si>
+    <t>Pan bearing inner cage</t>
+  </si>
+  <si>
+    <t>Pan bearing middle ring</t>
+  </si>
+  <si>
+    <t>Pan bearing outer cage</t>
+  </si>
+  <si>
+    <t>Pan bearing balls (4.5 mm)</t>
+  </si>
+  <si>
+    <t>M5x30 cap srew</t>
+  </si>
+  <si>
+    <t>Tilt rotor</t>
+  </si>
+  <si>
+    <t>byo/pantilt/panbearing</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_Pulley_17.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_motor_plate.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_motor_stop.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_Rotor_245.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_base.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_bearing_stop_bottom.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_bearing_stop_top.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_base.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_base_motor_side.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_Motor_pulley_20.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_Rotor_pulley_100.stl</t>
+  </si>
+  <si>
+    <t>Tilt rotor pulley</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_motor_spacer.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_bearing_stop.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_cover.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_tension_knot.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_bearing_inner.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_bearing_middle.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Pan_bearing_outter.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/Tilt_mirror_rotor.stl</t>
+  </si>
+  <si>
+    <t>byo/PanTilt/hot_mirror_holder.stl</t>
+  </si>
+  <si>
+    <t>1-st surface mirror, 101*127mm, 3mm thickness</t>
+  </si>
+  <si>
+    <t>high performance hot mirror (101x127mm) that only reflects IR</t>
+  </si>
+  <si>
+    <t>#64-462</t>
+  </si>
+  <si>
+    <t>Edmund</t>
+  </si>
+  <si>
+    <t>MB3060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluminum Breadboard, 300 mm x 600 mm x 12.7 mm, M6 Taps </t>
+  </si>
+  <si>
+    <t>M4x8 mm cap screw</t>
+  </si>
+  <si>
+    <t>M6x8 mm setscrew</t>
+  </si>
+  <si>
+    <t>ball head</t>
+  </si>
+  <si>
+    <t>M3x8 cap srew</t>
+  </si>
+  <si>
+    <t>M3x12 cap screw</t>
+  </si>
+  <si>
+    <t>M1.5x5 cap srew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 female insert </t>
+  </si>
+  <si>
+    <t>M3 female insert</t>
+  </si>
+  <si>
+    <t>heat by soldering iron and insert to the pan motor plate</t>
+  </si>
+  <si>
+    <t>heat by soldering iron and insert to the pan rotor</t>
+  </si>
+  <si>
+    <t>fixed pan bearing stoper top to pan base</t>
+  </si>
+  <si>
+    <t>mount tilt motor to tilt motor base</t>
+  </si>
+  <si>
+    <t>mount pan motor to pan motor plate and the tilt bases to pan rotor</t>
+  </si>
+  <si>
+    <t>pretty camera mount</t>
+  </si>
+  <si>
+    <t>mount all the posts to base plate</t>
+  </si>
+  <si>
+    <t>mount the pantilt head to the posts</t>
+  </si>
+  <si>
+    <t>M6 to 1/4"-20 adapter</t>
+  </si>
+  <si>
+    <t>mount ball head to post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">press fit to the pan tension knot and use for adjusting pan belt tesion </t>
+  </si>
+  <si>
+    <t>1/4"-20 cap srew</t>
+  </si>
+  <si>
+    <t>fix motor mount to the lens</t>
+  </si>
+  <si>
+    <t>61802-2RS</t>
+  </si>
+  <si>
+    <t>4.5 mm stainless steal ball insert to the pan bearing</t>
+  </si>
+  <si>
+    <t>laser cut</t>
+  </si>
+  <si>
+    <t>front cover</t>
+  </si>
+  <si>
+    <t>left cover</t>
+  </si>
+  <si>
+    <t>right corner cover</t>
+  </si>
+  <si>
+    <t>right cover</t>
+  </si>
+  <si>
+    <t>top right cover front</t>
+  </si>
+  <si>
+    <t>top right cover back</t>
+  </si>
+  <si>
+    <t>top cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do not cut through </t>
+  </si>
+  <si>
+    <t>tba</t>
+  </si>
+  <si>
+    <t>byo/focusing/ring_gear.stl</t>
+  </si>
+  <si>
+    <t>ball bearing 61802-2RS</t>
   </si>
 </sst>
 </file>
@@ -813,9 +1059,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -841,8 +1090,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}" name="Table1" displayName="Table1" ref="A9:L82" totalsRowShown="0">
-  <autoFilter ref="A9:L82" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}" name="Table1" displayName="Table1" ref="A9:L121" totalsRowShown="0">
+  <autoFilter ref="A9:L121" xr:uid="{854C557E-F3D9-4C6D-BE0C-6866F1D42822}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:L121">
+    <sortCondition ref="B9:B121"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{9442F240-FACF-48B0-A1BF-B6F8225D9FD1}" name="no"/>
     <tableColumn id="2" xr3:uid="{22CE39F6-6E8A-482E-97B6-A27252CDE540}" name="system"/>
@@ -1158,18 +1410,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25A315E-DF31-4262-87C2-ADD015BB9516}">
-  <dimension ref="A9:L82"/>
+  <dimension ref="A9:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
-    <col min="8" max="8" width="38.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="26.90625" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" style="1" customWidth="1"/>
     <col min="10" max="10" width="37.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="47.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.81640625" customWidth="1"/>
@@ -1210,1475 +1464,1353 @@
         <v>32</v>
       </c>
       <c r="L9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>110</v>
+      </c>
+      <c r="E10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" t="s">
+        <v>112</v>
       </c>
       <c r="G10">
         <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>16</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13">
-        <v>2000035953</v>
+        <v>312</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15">
-        <v>2200000315</v>
+        <v>82</v>
+      </c>
+      <c r="F15" t="s">
+        <v>104</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="J16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="J18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" t="s">
-        <v>41</v>
+        <v>244</v>
       </c>
       <c r="G19">
-        <v>24</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="J19" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" t="s">
-        <v>46</v>
+        <v>245</v>
       </c>
       <c r="G20">
-        <v>24</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="J20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H21" s="2"/>
+      <c r="J21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" t="s">
-        <v>52</v>
+        <v>247</v>
       </c>
       <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H22" s="2"/>
       <c r="J22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>248</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="K23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H23" s="2"/>
+      <c r="J23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H24" s="2"/>
+      <c r="J24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H25" s="2"/>
+      <c r="J25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" t="s">
-        <v>80</v>
+        <v>251</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H26" s="2"/>
+      <c r="J26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>252</v>
       </c>
       <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="J27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>65</v>
+        <v>243</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="J28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>65</v>
+        <v>243</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>254</v>
       </c>
       <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="J29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>243</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" t="s">
-        <v>72</v>
+        <v>255</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H30" s="2"/>
+      <c r="J30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" t="s">
-        <v>84</v>
+        <v>256</v>
       </c>
       <c r="G31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="J31" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>263</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>86</v>
+      <c r="H32" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
-      </c>
-      <c r="F33" t="s">
-        <v>92</v>
+        <v>257</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>245</v>
+      <c r="H33" s="2"/>
+      <c r="J33" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>258</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>314</v>
       </c>
       <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>244</v>
+        <v>2</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>81</v>
+        <v>243</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>264</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
+      <c r="H35" s="2"/>
       <c r="J35" t="s">
-        <v>88</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>277</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>96</v>
+      <c r="H36" s="2"/>
+      <c r="J36" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>296</v>
       </c>
       <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="J37" t="s">
-        <v>88</v>
+        <v>8</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
-      </c>
-      <c r="F38" t="s">
-        <v>98</v>
+        <v>297</v>
       </c>
       <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>99</v>
+        <v>4</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>298</v>
       </c>
       <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="J39" t="s">
-        <v>88</v>
+        <v>8</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E40" t="s">
-        <v>103</v>
-      </c>
-      <c r="F40" t="s">
-        <v>106</v>
+        <v>299</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>105</v>
+      <c r="H40" s="2" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" t="s">
-        <v>108</v>
+        <v>300</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>81</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" t="s">
+        <v>83</v>
       </c>
       <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J42" t="s">
-        <v>242</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
-      <c r="J43" t="s">
-        <v>243</v>
+      <c r="H43" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>89</v>
+      </c>
+      <c r="F44" t="s">
+        <v>91</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J44" t="s">
-        <v>88</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>101</v>
+        <v>243</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E45" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="F45" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="G45">
         <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>101</v>
+        <v>243</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>117</v>
-      </c>
-      <c r="E46" t="s">
-        <v>118</v>
-      </c>
-      <c r="F46" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="G46">
         <v>1</v>
+      </c>
+      <c r="J46" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>101</v>
+        <v>265</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
-      </c>
-      <c r="F47" t="s">
-        <v>88</v>
+        <v>259</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>88</v>
+      <c r="H47" s="2"/>
+      <c r="J47" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>93</v>
+        <v>265</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s">
-        <v>121</v>
-      </c>
-      <c r="F48" t="s">
-        <v>88</v>
+        <v>260</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H48" s="2"/>
+      <c r="J48" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>93</v>
+        <v>265</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" t="s">
-        <v>123</v>
+        <v>261</v>
       </c>
       <c r="G49">
-        <v>4</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="J49" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>93</v>
+        <v>265</v>
       </c>
       <c r="C50" t="s">
         <v>29</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" t="s">
-        <v>125</v>
+        <v>262</v>
       </c>
       <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
         <v>29</v>
       </c>
       <c r="D51" t="s">
-        <v>122</v>
+        <v>309</v>
       </c>
       <c r="E51" t="s">
         <v>26</v>
       </c>
-      <c r="F51" t="s">
-        <v>126</v>
-      </c>
       <c r="G51">
-        <v>2</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>295</v>
       </c>
       <c r="E52" t="s">
         <v>26</v>
       </c>
-      <c r="F52" t="s">
-        <v>129</v>
-      </c>
       <c r="G52">
         <v>1</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H52" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>122</v>
-      </c>
-      <c r="E53" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" t="s">
-        <v>130</v>
+        <v>294</v>
       </c>
       <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" t="s">
         <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
-      </c>
-      <c r="E54" t="s">
+        <v>293</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" t="s">
+        <v>93</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="J56" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" t="s">
+        <v>290</v>
+      </c>
+      <c r="F57" t="s">
+        <v>289</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" t="s">
+        <v>96</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="J58" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" t="s">
+        <v>117</v>
+      </c>
+      <c r="E59" t="s">
         <v>26</v>
       </c>
-      <c r="F54" t="s">
-        <v>133</v>
-      </c>
-      <c r="G54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="F59" t="s">
+        <v>291</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" t="s">
         <v>29</v>
       </c>
-      <c r="D55" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E60" t="s">
         <v>26</v>
       </c>
-      <c r="F55" t="s">
-        <v>136</v>
-      </c>
-      <c r="G55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="F60" t="s">
+        <v>119</v>
+      </c>
+      <c r="G60">
+        <v>4</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" t="s">
         <v>29</v>
       </c>
-      <c r="D56" t="s">
-        <v>138</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D61" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" t="s">
         <v>26</v>
       </c>
-      <c r="F56" t="s">
-        <v>137</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>181</v>
-      </c>
-      <c r="C57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" t="s">
-        <v>139</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K57" t="s">
-        <v>61</v>
-      </c>
-      <c r="L57" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>182</v>
-      </c>
-      <c r="C58" t="s">
-        <v>39</v>
-      </c>
-      <c r="D58" t="s">
-        <v>140</v>
-      </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K58" t="s">
-        <v>61</v>
-      </c>
-      <c r="L58" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" t="s">
-        <v>39</v>
-      </c>
-      <c r="D59" t="s">
-        <v>141</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="K59" t="s">
-        <v>61</v>
-      </c>
-      <c r="L59" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B60" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" t="s">
-        <v>39</v>
-      </c>
-      <c r="D60" t="s">
-        <v>142</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="K60" t="s">
-        <v>61</v>
-      </c>
-      <c r="L60" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
-        <v>185</v>
-      </c>
-      <c r="C61" t="s">
-        <v>39</v>
-      </c>
-      <c r="D61" t="s">
-        <v>143</v>
+      <c r="F61" t="s">
+        <v>121</v>
       </c>
       <c r="G61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="K61" t="s">
-        <v>61</v>
-      </c>
-      <c r="L61" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D62" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
+        <v>26</v>
       </c>
       <c r="F62" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
       <c r="G62">
         <v>2</v>
       </c>
-      <c r="K62" t="s">
-        <v>61</v>
-      </c>
-      <c r="L62" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H62" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>187</v>
+        <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="F63" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" t="s">
+        <v>126</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>129</v>
+      </c>
+      <c r="G65">
         <v>3</v>
       </c>
-      <c r="K63" t="s">
-        <v>61</v>
-      </c>
-      <c r="L63" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
-        <v>188</v>
-      </c>
-      <c r="C64" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64" t="s">
-        <v>146</v>
-      </c>
-      <c r="G64">
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
+        <v>132</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" t="s">
+        <v>133</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" t="s">
+        <v>316</v>
+      </c>
+      <c r="D68" t="s">
+        <v>317</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" s="2"/>
+      <c r="J68" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" t="s">
+        <v>316</v>
+      </c>
+      <c r="D69" t="s">
+        <v>318</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" s="2"/>
+      <c r="J69" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" t="s">
+        <v>316</v>
+      </c>
+      <c r="D70" t="s">
+        <v>319</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" s="2"/>
+      <c r="J70" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" t="s">
+        <v>316</v>
+      </c>
+      <c r="D71" t="s">
+        <v>320</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>324</v>
+      </c>
+      <c r="J71" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>316</v>
+      </c>
+      <c r="D72" t="s">
+        <v>321</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" s="2"/>
+      <c r="J72" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>92</v>
+      </c>
+      <c r="C73" t="s">
+        <v>316</v>
+      </c>
+      <c r="D73" t="s">
+        <v>322</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73" s="2"/>
+      <c r="J73" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>92</v>
+      </c>
+      <c r="C74" t="s">
+        <v>316</v>
+      </c>
+      <c r="D74" t="s">
+        <v>323</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" s="2"/>
+      <c r="J74" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>34</v>
+      </c>
+      <c r="F75" t="s">
+        <v>35</v>
+      </c>
+      <c r="G75">
         <v>2</v>
       </c>
-      <c r="K64" t="s">
-        <v>61</v>
-      </c>
-      <c r="L64" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
-        <v>189</v>
-      </c>
-      <c r="C65" t="s">
-        <v>39</v>
-      </c>
-      <c r="D65" t="s">
-        <v>147</v>
-      </c>
-      <c r="E65" t="s">
-        <v>240</v>
-      </c>
-      <c r="F65" t="s">
-        <v>167</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="K65" t="s">
-        <v>61</v>
-      </c>
-      <c r="L65" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
-        <v>190</v>
-      </c>
-      <c r="C66" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" t="s">
-        <v>148</v>
-      </c>
-      <c r="G66">
-        <v>2</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="K66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L66" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
-        <v>191</v>
-      </c>
-      <c r="C67" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" t="s">
-        <v>149</v>
-      </c>
-      <c r="G67">
-        <v>2</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="K67" t="s">
-        <v>61</v>
-      </c>
-      <c r="L67" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
-        <v>192</v>
-      </c>
-      <c r="C68" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" t="s">
-        <v>150</v>
-      </c>
-      <c r="E68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F68" t="s">
-        <v>168</v>
-      </c>
-      <c r="G68">
-        <v>1</v>
-      </c>
-      <c r="K68" t="s">
-        <v>61</v>
-      </c>
-      <c r="L68" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B69" t="s">
-        <v>193</v>
-      </c>
-      <c r="C69" t="s">
-        <v>39</v>
-      </c>
-      <c r="D69" t="s">
-        <v>151</v>
-      </c>
-      <c r="E69" t="s">
-        <v>176</v>
-      </c>
-      <c r="F69" t="s">
-        <v>169</v>
-      </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="K69" t="s">
-        <v>61</v>
-      </c>
-      <c r="L69" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
-        <v>194</v>
-      </c>
-      <c r="C70" t="s">
-        <v>39</v>
-      </c>
-      <c r="D70" t="s">
-        <v>152</v>
-      </c>
-      <c r="G70">
-        <v>1</v>
-      </c>
-      <c r="K70" t="s">
-        <v>61</v>
-      </c>
-      <c r="L70" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
-        <v>195</v>
-      </c>
-      <c r="C71" t="s">
-        <v>39</v>
-      </c>
-      <c r="D71" t="s">
-        <v>153</v>
-      </c>
-      <c r="G71">
-        <v>1</v>
-      </c>
-      <c r="K71" t="s">
-        <v>61</v>
-      </c>
-      <c r="L71" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
-        <v>196</v>
-      </c>
-      <c r="C72" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72" t="s">
-        <v>154</v>
-      </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-      <c r="K72" t="s">
-        <v>61</v>
-      </c>
-      <c r="L72" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B73" t="s">
-        <v>197</v>
-      </c>
-      <c r="C73" t="s">
-        <v>39</v>
-      </c>
-      <c r="D73" t="s">
-        <v>155</v>
-      </c>
-      <c r="E73" t="s">
-        <v>177</v>
-      </c>
-      <c r="F73" t="s">
-        <v>170</v>
-      </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
-      <c r="K73" t="s">
-        <v>61</v>
-      </c>
-      <c r="L73" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
-        <v>198</v>
-      </c>
-      <c r="C74" t="s">
-        <v>39</v>
-      </c>
-      <c r="D74" t="s">
-        <v>156</v>
-      </c>
-      <c r="G74">
-        <v>4</v>
-      </c>
-      <c r="K74" t="s">
-        <v>61</v>
-      </c>
-      <c r="L74" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>199</v>
-      </c>
-      <c r="C75" t="s">
-        <v>39</v>
-      </c>
-      <c r="D75" t="s">
-        <v>157</v>
-      </c>
-      <c r="G75">
-        <v>9</v>
+      <c r="H75" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="K75" t="s">
-        <v>61</v>
-      </c>
-      <c r="L75" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="C76" t="s">
         <v>39</v>
       </c>
       <c r="D76" t="s">
-        <v>158</v>
+        <v>43</v>
+      </c>
+      <c r="E76" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" t="s">
+        <v>41</v>
       </c>
       <c r="G76">
-        <v>2</v>
-      </c>
-      <c r="K76" t="s">
-        <v>61</v>
-      </c>
-      <c r="L76" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>201</v>
+        <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>159</v>
+        <v>44</v>
+      </c>
+      <c r="E77" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" t="s">
+        <v>46</v>
       </c>
       <c r="G77">
-        <v>1</v>
-      </c>
-      <c r="K77" t="s">
-        <v>61</v>
-      </c>
-      <c r="L77" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
       <c r="C78" t="s">
         <v>39</v>
       </c>
       <c r="D78" t="s">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="G78">
         <v>1</v>
       </c>
-      <c r="K78" t="s">
-        <v>61</v>
-      </c>
-      <c r="L78" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="H78" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>203</v>
+        <v>48</v>
       </c>
       <c r="C79" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D79" t="s">
-        <v>161</v>
-      </c>
-      <c r="E79" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="F79" t="s">
-        <v>161</v>
+        <v>52</v>
       </c>
       <c r="G79">
-        <v>1</v>
-      </c>
-      <c r="K79" t="s">
-        <v>61</v>
-      </c>
-      <c r="L79" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J79" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>204</v>
+        <v>55</v>
       </c>
       <c r="C80" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D80" t="s">
-        <v>162</v>
-      </c>
-      <c r="E80" t="s">
-        <v>179</v>
-      </c>
-      <c r="F80" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -2686,60 +2818,888 @@
       <c r="K80" t="s">
         <v>61</v>
       </c>
-      <c r="L80" t="s">
-        <v>237</v>
-      </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>205</v>
+        <v>55</v>
       </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D81" t="s">
-        <v>163</v>
+        <v>62</v>
       </c>
       <c r="E81" t="s">
-        <v>179</v>
+        <v>74</v>
       </c>
       <c r="F81" t="s">
-        <v>172</v>
+        <v>75</v>
       </c>
       <c r="G81">
         <v>1</v>
       </c>
-      <c r="K81" t="s">
-        <v>61</v>
-      </c>
-      <c r="L81" t="s">
-        <v>238</v>
+      <c r="H81" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
+        <v>55</v>
+      </c>
+      <c r="C82" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" t="s">
+        <v>76</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" t="s">
+        <v>56</v>
+      </c>
+      <c r="D83" t="s">
+        <v>64</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D84" t="s">
+        <v>143</v>
+      </c>
+      <c r="E84" t="s">
+        <v>236</v>
+      </c>
+      <c r="F84" t="s">
+        <v>163</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="K84" t="s">
+        <v>61</v>
+      </c>
+      <c r="L84" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" t="s">
+        <v>144</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K85" t="s">
+        <v>61</v>
+      </c>
+      <c r="L85" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" t="s">
+        <v>145</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K86" t="s">
+        <v>61</v>
+      </c>
+      <c r="L86" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" t="s">
+        <v>146</v>
+      </c>
+      <c r="E87" t="s">
+        <v>79</v>
+      </c>
+      <c r="F87" t="s">
+        <v>164</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>61</v>
+      </c>
+      <c r="L87" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>189</v>
+      </c>
+      <c r="C88" t="s">
+        <v>39</v>
+      </c>
+      <c r="D88" t="s">
+        <v>147</v>
+      </c>
+      <c r="E88" t="s">
+        <v>172</v>
+      </c>
+      <c r="F88" t="s">
+        <v>165</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="K88" t="s">
+        <v>61</v>
+      </c>
+      <c r="L88" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>190</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D89" t="s">
+        <v>148</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="K89" t="s">
+        <v>61</v>
+      </c>
+      <c r="L89" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D90" t="s">
+        <v>149</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="K90" t="s">
+        <v>61</v>
+      </c>
+      <c r="L90" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" t="s">
+        <v>150</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="K91" t="s">
+        <v>61</v>
+      </c>
+      <c r="L91" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" t="s">
+        <v>39</v>
+      </c>
+      <c r="D92" t="s">
+        <v>151</v>
+      </c>
+      <c r="E92" t="s">
+        <v>173</v>
+      </c>
+      <c r="F92" t="s">
+        <v>166</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="K92" t="s">
+        <v>61</v>
+      </c>
+      <c r="L92" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93" t="s">
+        <v>152</v>
+      </c>
+      <c r="G93">
+        <v>4</v>
+      </c>
+      <c r="K93" t="s">
+        <v>61</v>
+      </c>
+      <c r="L93" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>177</v>
+      </c>
+      <c r="C94" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" t="s">
+        <v>135</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K94" t="s">
+        <v>61</v>
+      </c>
+      <c r="L94" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95" t="s">
+        <v>153</v>
+      </c>
+      <c r="G95">
+        <v>9</v>
+      </c>
+      <c r="K95" t="s">
+        <v>61</v>
+      </c>
+      <c r="L95" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" t="s">
+        <v>154</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+      <c r="K96" t="s">
+        <v>61</v>
+      </c>
+      <c r="L96" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B97" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" t="s">
+        <v>39</v>
+      </c>
+      <c r="D97" t="s">
+        <v>155</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="K97" t="s">
+        <v>61</v>
+      </c>
+      <c r="L97" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>198</v>
+      </c>
+      <c r="C98" t="s">
+        <v>39</v>
+      </c>
+      <c r="D98" t="s">
+        <v>156</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="K98" t="s">
+        <v>61</v>
+      </c>
+      <c r="L98" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B99" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" t="s">
+        <v>157</v>
+      </c>
+      <c r="E99" t="s">
+        <v>174</v>
+      </c>
+      <c r="F99" t="s">
+        <v>157</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="K99" t="s">
+        <v>61</v>
+      </c>
+      <c r="L99" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B100" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" t="s">
+        <v>158</v>
+      </c>
+      <c r="E100" t="s">
+        <v>175</v>
+      </c>
+      <c r="F100" t="s">
+        <v>167</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="K100" t="s">
+        <v>61</v>
+      </c>
+      <c r="L100" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>201</v>
+      </c>
+      <c r="C101" t="s">
+        <v>39</v>
+      </c>
+      <c r="D101" t="s">
+        <v>159</v>
+      </c>
+      <c r="E101" t="s">
+        <v>175</v>
+      </c>
+      <c r="F101" t="s">
+        <v>168</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="K101" t="s">
+        <v>61</v>
+      </c>
+      <c r="L101" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D102" t="s">
+        <v>160</v>
+      </c>
+      <c r="E102" t="s">
+        <v>176</v>
+      </c>
+      <c r="F102" t="s">
+        <v>169</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="K102" t="s">
+        <v>61</v>
+      </c>
+      <c r="L102" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B103" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" t="s">
+        <v>39</v>
+      </c>
+      <c r="D103" t="s">
+        <v>136</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K103" t="s">
+        <v>61</v>
+      </c>
+      <c r="L103" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B104" t="s">
+        <v>179</v>
+      </c>
+      <c r="C104" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" t="s">
+        <v>137</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="K104" t="s">
+        <v>61</v>
+      </c>
+      <c r="L104" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B105" t="s">
+        <v>180</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" t="s">
+        <v>138</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K105" t="s">
+        <v>61</v>
+      </c>
+      <c r="L105" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B106" t="s">
+        <v>181</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+      <c r="D106" t="s">
+        <v>139</v>
+      </c>
+      <c r="G106">
+        <v>2</v>
+      </c>
+      <c r="H106" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C82" t="s">
+      <c r="K106" t="s">
+        <v>61</v>
+      </c>
+      <c r="L106" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B107" t="s">
+        <v>182</v>
+      </c>
+      <c r="C107" t="s">
         <v>39</v>
       </c>
-      <c r="D82" t="s">
-        <v>164</v>
-      </c>
-      <c r="E82" t="s">
-        <v>180</v>
-      </c>
-      <c r="F82" t="s">
-        <v>173</v>
-      </c>
-      <c r="G82">
-        <v>1</v>
-      </c>
-      <c r="K82" t="s">
+      <c r="D107" t="s">
+        <v>140</v>
+      </c>
+      <c r="E107" t="s">
+        <v>170</v>
+      </c>
+      <c r="F107" t="s">
+        <v>161</v>
+      </c>
+      <c r="G107">
+        <v>2</v>
+      </c>
+      <c r="K107" t="s">
         <v>61</v>
       </c>
-      <c r="L82" t="s">
-        <v>239</v>
+      <c r="L107" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>183</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" t="s">
+        <v>141</v>
+      </c>
+      <c r="E108" t="s">
+        <v>171</v>
+      </c>
+      <c r="F108" t="s">
+        <v>162</v>
+      </c>
+      <c r="G108">
+        <v>3</v>
+      </c>
+      <c r="K108" t="s">
+        <v>61</v>
+      </c>
+      <c r="L108" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
+        <v>184</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+      <c r="D109" t="s">
+        <v>142</v>
+      </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+      <c r="K109" t="s">
+        <v>61</v>
+      </c>
+      <c r="L109" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B110" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+      <c r="D110" t="s">
+        <v>66</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" t="s">
+        <v>67</v>
+      </c>
+      <c r="G111">
+        <v>2</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B112" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D112" t="s">
+        <v>68</v>
+      </c>
+      <c r="E112" t="s">
+        <v>73</v>
+      </c>
+      <c r="F112" t="s">
+        <v>72</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B113" t="s">
+        <v>77</v>
+      </c>
+      <c r="C113" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" t="s">
+        <v>78</v>
+      </c>
+      <c r="E113" t="s">
+        <v>79</v>
+      </c>
+      <c r="F113" t="s">
+        <v>80</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" t="s">
+        <v>31</v>
+      </c>
+      <c r="D114" t="s">
+        <v>28</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="J114" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
+        <v>13</v>
+      </c>
+      <c r="C115" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" t="s">
+        <v>23</v>
+      </c>
+      <c r="F115" t="s">
+        <v>24</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" t="s">
+        <v>30</v>
+      </c>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" t="s">
+        <v>25</v>
+      </c>
+      <c r="F116" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B117" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" t="s">
+        <v>29</v>
+      </c>
+      <c r="D117" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" t="s">
+        <v>23</v>
+      </c>
+      <c r="F117">
+        <v>2000035953</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B118" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" t="s">
+        <v>56</v>
+      </c>
+      <c r="D118" t="s">
+        <v>57</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B119" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119" t="s">
+        <v>56</v>
+      </c>
+      <c r="D119" t="s">
+        <v>59</v>
+      </c>
+      <c r="E119" t="s">
+        <v>23</v>
+      </c>
+      <c r="F119">
+        <v>2200000315</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B120" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" t="s">
+        <v>30</v>
+      </c>
+      <c r="D120" t="s">
+        <v>20</v>
+      </c>
+      <c r="E120" t="s">
+        <v>26</v>
+      </c>
+      <c r="F120" t="s">
+        <v>21</v>
+      </c>
+      <c r="G120">
+        <v>2</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D121" t="s">
+        <v>7</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bom: refine ball head
</commit_message>
<xml_diff>
--- a/byo/bom.xlsx
+++ b/byo/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\_vt\strawlab\projects\flo-hardware\byo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8462B8-DEAF-47EE-8E50-C60FCEAFA7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4B3A36-BD5B-4CD8-AB0F-E2FC32944317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
+    <workbookView xWindow="580" yWindow="3330" windowWidth="24570" windowHeight="10680" xr2:uid="{DB374029-A34F-43BD-A740-E6CE7544A665}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="321">
   <si>
     <t>no</t>
   </si>
@@ -991,6 +991,12 @@
   </si>
   <si>
     <t>A to micro-B 3 meters, connect steppers to pc</t>
+  </si>
+  <si>
+    <t>Giottos</t>
+  </si>
+  <si>
+    <t>MH1004</t>
   </si>
 </sst>
 </file>
@@ -1032,12 +1038,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1385,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25A315E-DF31-4262-87C2-ADD015BB9516}">
   <dimension ref="A9:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1499,7 +1502,7 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>274</v>
       </c>
     </row>
@@ -1516,7 +1519,7 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>277</v>
       </c>
     </row>
@@ -1531,7 +1534,10 @@
         <v>263</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>319</v>
+      </c>
+      <c r="F14" t="s">
+        <v>320</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1650,7 +1656,7 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>296</v>
       </c>
     </row>
@@ -1707,7 +1713,7 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3337,7 +3343,7 @@
       <c r="G103">
         <v>2</v>
       </c>
-      <c r="H103" s="2" t="s">
+      <c r="H103" s="1" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3374,7 +3380,7 @@
       <c r="G105">
         <v>2</v>
       </c>
-      <c r="H105" s="2" t="s">
+      <c r="H105" s="1" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3397,7 +3403,7 @@
       <c r="G106">
         <v>2</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="H106" s="1" t="s">
         <v>316</v>
       </c>
     </row>

</xml_diff>